<commit_message>
Fix definition in SBER
</commit_message>
<xml_diff>
--- a/sources/SBER/tables/sber.xlsx
+++ b/sources/SBER/tables/sber.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t xml:space="preserve">Год</t>
   </si>
@@ -30,112 +30,115 @@
     <t xml:space="preserve">LTM</t>
   </si>
   <si>
+    <t xml:space="preserve">Операционные доходы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Прибыль до налогообложения</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Налог на прибыль</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Чистая прибыль</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Активы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Капитал</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Обязательства</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Налог на прибыль, %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Количество акций</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Цена акции</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Капитализация</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P/E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P/BV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дивиденды на акцию</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Доля собственного капитала</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Доля заёмного капитала</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Безрисковая ставка, ОФЗ на 10 лет (Rf)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Средняя доходность фондового рынка (Rm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">β</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Стоимость акционерного капитала (Re)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Стоимость долгового капитала (Rd)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WACC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAGR \ лет</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Выручка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Валовая прибыль</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EBITDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Амортизация/Выручка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capex/Выручка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Оборотный капитал/Выручка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Амортизация</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Оборотный капитал</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Изменение оборотного капитала</t>
+  </si>
+  <si>
     <t xml:space="preserve">Операционная прибыль</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Прибыль до налогообложения</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Налог на прибыль</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Чистая прибыль</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Активы</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Капитал</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Обязательства</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Налог на прибыль, %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Количество акций</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Цена акции</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Капитализация</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P/E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P/BV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Дивиденды на акцию</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Доля собственного капитала</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Доля заёмного капитала</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Безрисковая ставка, ОФЗ на 10 лет (Rf)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Средняя доходность фондового рынка (Rm)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">β</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Стоимость акционерного капитала (Re)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Стоимость долгового капитала (Rd)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WACC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAGR \ лет</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Выручка</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Валовая прибыль</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EBITDA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Амортизация/Выручка</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capex/Выручка</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Оборотный капитал/Выручка</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Амортизация</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Оборотный капитал</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Изменение оборотного капитала</t>
   </si>
   <si>
     <t xml:space="preserve">FCF</t>
@@ -157,14 +160,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="#,##0\ [$₽-419];[RED]\-#,##0\ [$₽-419]"/>
     <numFmt numFmtId="167" formatCode="0.00%"/>
     <numFmt numFmtId="168" formatCode="#,##0.00"/>
     <numFmt numFmtId="169" formatCode="#,##0.00\ [$₽-419];[RED]\-#,##0.00\ [$₽-419]"/>
-    <numFmt numFmtId="170" formatCode="#,##0.00\ [$₽-419];[RED]\-#,##0.00\ [$₽-419]"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -304,7 +306,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -385,39 +387,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -546,10 +516,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="2" width="19.71"/>
@@ -1081,145 +1051,142 @@
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="20" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-    </row>
-    <row r="21" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="20"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-    </row>
-    <row r="22" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="20"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-    </row>
-    <row r="26" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="24"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-    </row>
-    <row r="27" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="24"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-    </row>
-    <row r="28" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="20"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-    </row>
-    <row r="29" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="24"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-    </row>
-    <row r="30" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="20"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-    </row>
-    <row r="31" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="20"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-    </row>
-    <row r="32" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="20"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-    </row>
-    <row r="33" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="20"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-    </row>
-    <row r="34" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="20"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-    </row>
-    <row r="37" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="20"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
-    </row>
-    <row r="40" s="30" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="9"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="26" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="9"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="9"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+    </row>
+    <row r="32" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="9"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+    </row>
+    <row r="33" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+    </row>
+    <row r="34" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="9"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="9"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+    </row>
+    <row r="40" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1240,59 +1207,59 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="39.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="39.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="33" t="n">
+      <c r="B1" s="25" t="n">
         <f aca="false">Data!$B$8/Data!$B$6</f>
         <v>0.861945461481958</v>
       </c>
     </row>
-    <row r="2" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="32" t="s">
+    <row r="2" s="25" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="33" t="n">
+      <c r="B2" s="25" t="n">
         <f aca="false">1-B1</f>
         <v>0.138054538518042</v>
       </c>
     </row>
-    <row r="3" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="31" t="s">
+    <row r="3" s="25" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="33" t="n">
+      <c r="B3" s="25" t="n">
         <f aca="false">Data!$B$9</f>
         <v>0.20482428779372</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="33" t="n">
+      <c r="B4" s="25" t="n">
         <v>0.056</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="33" t="n">
+      <c r="B5" s="25" t="n">
         <v>0.198</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="26" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="4" t="n">
@@ -1300,145 +1267,145 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="33" t="n">
+      <c r="B7" s="25" t="n">
         <f aca="false">B4+B6*(B5-B4)</f>
         <v>0.08014</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="33" t="n">
+      <c r="B8" s="25" t="n">
         <v>0.0898</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="33" t="n">
+      <c r="B9" s="25" t="n">
         <f aca="false">B1*B7+B2*B8*(1-B3)</f>
         <v>0.0789343391990116</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="36" t="n">
+      <c r="B11" s="28" t="n">
         <v>6</v>
       </c>
-      <c r="C11" s="36" t="n">
+      <c r="C11" s="28" t="n">
         <f aca="false">B11-1</f>
         <v>5</v>
       </c>
-      <c r="D11" s="36" t="n">
+      <c r="D11" s="28" t="n">
         <f aca="false">C11-1</f>
         <v>4</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="33" t="n">
+      <c r="B12" s="25" t="n">
         <f aca="false">(Data!$B$2/Data!$H$2)^(1/$B$11) - 1</f>
         <v>0.10574957142703</v>
       </c>
-      <c r="C12" s="33" t="n">
+      <c r="C12" s="25" t="n">
         <f aca="false">(Data!$B$2/Data!$G$2)^(1/$C$11) - 1</f>
         <v>0.124565391896789</v>
       </c>
-      <c r="D12" s="33" t="n">
+      <c r="D12" s="25" t="n">
         <f aca="false">(Data!$B$2/Data!$F$2)^(1/$D$11) - 1</f>
         <v>0.0609463275498428</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="33" t="n">
+      <c r="B13" s="25" t="n">
         <f aca="false">(Data!$B$4/Data!$H$4)^(1/$B$11) - 1</f>
         <v>0.152879838208101</v>
       </c>
-      <c r="C13" s="33" t="n">
+      <c r="C13" s="25" t="n">
         <f aca="false">(Data!$B$4/Data!$G$4)^(1/$C$11) - 1</f>
         <v>0.127113246523822</v>
       </c>
-      <c r="D13" s="33" t="n">
+      <c r="D13" s="25" t="n">
         <f aca="false">(Data!$B$4/Data!$F$4)^(1/$D$11) - 1</f>
         <v>0.0978718107357019</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="33" t="e">
+      <c r="B14" s="25" t="e">
         <f aca="false">(Data!$B$32/Data!$H$32)^(1/$B$11) - 1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C14" s="33" t="e">
+      <c r="C14" s="25" t="e">
         <f aca="false">(Data!$B$32/Data!$G$32)^(1/$C$11) - 1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D14" s="33" t="e">
+      <c r="D14" s="25" t="e">
         <f aca="false">(Data!$B$32/Data!$F$32)^(1/$D$11) - 1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="33" t="n">
+      <c r="B15" s="25" t="n">
         <f aca="false">((Data!$B$18/Data!$B$2)/(Data!$H$18/Data!$H$2))^(1/$B$11) - 1</f>
         <v>0.213738584579527</v>
       </c>
-      <c r="C15" s="33" t="n">
+      <c r="C15" s="25" t="n">
         <f aca="false">((Data!$B$18/Data!$B$2)/(Data!$G$18/Data!$G$2))^(1/$C$11) - 1</f>
         <v>0.873877102419684</v>
       </c>
-      <c r="D15" s="33" t="n">
+      <c r="D15" s="25" t="n">
         <f aca="false">((Data!$B$18/Data!$B$2)/(Data!$F$18/Data!$F$2))^(1/$D$11) - 1</f>
         <v>0.65443775095519</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="33" t="n">
+      <c r="B16" s="25" t="n">
         <f aca="false">((Data!$B$10/Data!$B$2)/(Data!$H$10/Data!$H$2))^(1/$B$11) - 1</f>
         <v>-0.109188944337511</v>
       </c>
-      <c r="C16" s="33" t="n">
+      <c r="C16" s="25" t="n">
         <f aca="false">((Data!$B$10/Data!$B$2)/(Data!$G$10/Data!$G$2))^(1/$C$11) - 1</f>
         <v>-0.0279040786028633</v>
       </c>
-      <c r="D16" s="33" t="n">
+      <c r="D16" s="25" t="n">
         <f aca="false">((Data!$B$10/Data!$B$2)/(Data!$F$10/Data!$F$2))^(1/$D$11) - 1</f>
         <v>-0.0493521281274802</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="33" t="e">
+      <c r="B17" s="25" t="e">
         <f aca="false">((Data!$B$20/Data!$B$2)/(Data!$H$20/Data!$H$2))^(1/$B$11) - 1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C17" s="33" t="e">
+      <c r="C17" s="25" t="e">
         <f aca="false">((Data!$B$20/Data!$B$2)/(Data!$G$20/Data!$G$2))^(1/$C$11) - 1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D17" s="33" t="e">
+      <c r="D17" s="25" t="e">
         <f aca="false">((Data!$B$20/Data!$B$2)/(Data!$F$20/Data!$F$2))^(1/$D$11) - 1</f>
         <v>#DIV/0!</v>
       </c>
@@ -1465,7 +1432,7 @@
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="28.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="4" width="17.86"/>
@@ -1737,7 +1704,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="B9" s="8" t="n">
         <f aca="false">B4-B5</f>
@@ -1770,7 +1737,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10" s="8" t="n">
         <f aca="false">B9*(1-AnalysisVals!$B$3)+B5-B8-B6</f>
@@ -1796,14 +1763,14 @@
         <f aca="false">(G9*(1-AnalysisVals!$B$3)+G5-G8-G6)/( (1+AnalysisVals!$B$9)^COUNT($C1:G1) )</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H10" s="38" t="n">
+      <c r="H10" s="30" t="n">
         <f aca="false">Data!$B$31/( (1-AnalysisVals!$B$8)^COUNT(C1:G1) )</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>34</v>
@@ -1811,9 +1778,9 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="33" t="n">
+        <v>41</v>
+      </c>
+      <c r="B13" s="25" t="n">
         <v>0.01</v>
       </c>
       <c r="C13" s="19" t="e">
@@ -1823,7 +1790,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" s="8" t="e">
         <f aca="false">SUM(B10:H10)/Data!$B$11</f>
@@ -1832,7 +1799,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" s="8" t="n">
         <v>1306</v>

</xml_diff>